<commit_message>
updates output file maker and files to reflect most recent paradigm
</commit_message>
<xml_diff>
--- a/runs/run010/NotionalETEOutput010.xlsx
+++ b/runs/run010/NotionalETEOutput010.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwhite\OneDrive - Torch Technologies, Inc\etesim_gui_test\runs\run010\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_EB72C09AACD72BEB61FD9890E22D62B190B42066" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9F751C76-8037-4102-B224-0E98C6E705C4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -55,20 +49,20 @@
     <t>tUp</t>
   </si>
   <si>
-    <t>Missile_HIGHWIND2_State_Update</t>
+    <t>Missile_ANGERMAX2_State_Update</t>
   </si>
   <si>
-    <t>MISSILE_HIGHWIND2_306.MISSILE_HIGHWIND2_306</t>
+    <t>MISSILE_ANGERMAX2_468.MISSILE_ANGERMAX2_468</t>
   </si>
   <si>
-    <t>MISSILE_HIGHWIND2</t>
+    <t>MISSILE_ANGERMAX2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,14 +125,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -185,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,27 +203,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,24 +237,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -462,19 +412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>10</v>
       </c>
@@ -535,16 +480,16 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>-1435.7084032992791</v>
+        <v>-1573.587032882787</v>
       </c>
       <c r="J2">
-        <v>2053.4044543944019</v>
+        <v>2032.167819573139</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>10</v>
       </c>
@@ -570,16 +515,16 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>-1517.725017452165</v>
+        <v>-1455.179115140841</v>
       </c>
       <c r="J3">
-        <v>1969.8462838044959</v>
+        <v>1974.576415652925</v>
       </c>
       <c r="K3">
-        <v>292.79407853758141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>316.2800275016236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>10</v>
       </c>
@@ -605,16 +550,16 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>-1418.572246496288</v>
+        <v>-1434.1253606197</v>
       </c>
       <c r="J4">
-        <v>1840.362889194522</v>
+        <v>1965.595796181476</v>
       </c>
       <c r="K4">
-        <v>616.00622132288549</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>583.1639455503765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>10</v>
       </c>
@@ -640,16 +585,16 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>-1473.9260013541621</v>
+        <v>-1417.402595217621</v>
       </c>
       <c r="J5">
-        <v>1772.0004690247699</v>
+        <v>1851.395202956704</v>
       </c>
       <c r="K5">
-        <v>894.9429082527605</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>848.6903663704209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>10</v>
       </c>
@@ -675,16 +620,16 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>-1386.1693073744821</v>
+        <v>-1428.054747359177</v>
       </c>
       <c r="J6">
-        <v>1840.120327868008</v>
+        <v>1844.057257215934</v>
       </c>
       <c r="K6">
-        <v>1081.9583474947431</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1130.040382356711</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>10</v>
       </c>
@@ -710,16 +655,16 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>-1303.3555231822379</v>
+        <v>-1407.631118172161</v>
       </c>
       <c r="J7">
-        <v>1830.3566075294989</v>
+        <v>1786.859289519137</v>
       </c>
       <c r="K7">
-        <v>1301.6345470224221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1322.405336220726</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>10</v>
       </c>
@@ -745,16 +690,16 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>-1290.8979941111049</v>
+        <v>-1284.854029251887</v>
       </c>
       <c r="J8">
-        <v>1746.367289687307</v>
+        <v>1673.859871536685</v>
       </c>
       <c r="K8">
-        <v>1573.4728444966099</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1525.360931848673</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>10</v>
       </c>
@@ -774,22 +719,22 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>-98.444942761716675</v>
+        <v>-104.9032508153096</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>-1280.17375707169</v>
+        <v>-1319.334413323036</v>
       </c>
       <c r="J9">
-        <v>1736.7961016586819</v>
+        <v>1706.634834989053</v>
       </c>
       <c r="K9">
-        <v>1735.241803044305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1875.692663536948</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>10</v>
       </c>
@@ -806,25 +751,25 @@
         <v>160.142</v>
       </c>
       <c r="F10">
-        <v>210.93456096346699</v>
+        <v>213.4861827150019</v>
       </c>
       <c r="G10">
-        <v>-87.656025874237002</v>
+        <v>-83.82353477443741</v>
       </c>
       <c r="H10">
-        <v>823.44908473489204</v>
+        <v>878.6023749890238</v>
       </c>
       <c r="I10">
-        <v>-1192.7636875046651</v>
+        <v>-1280.302969319163</v>
       </c>
       <c r="J10">
-        <v>1586.3974401950891</v>
+        <v>1583.506362198231</v>
       </c>
       <c r="K10">
-        <v>1936.639617659172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1942.979460160965</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
@@ -841,25 +786,25 @@
         <v>161.142</v>
       </c>
       <c r="F11">
-        <v>168.16754633633639</v>
+        <v>170.129049217227</v>
       </c>
       <c r="G11">
-        <v>-66.97891571991218</v>
+        <v>-64.89130889164315</v>
       </c>
       <c r="H11">
-        <v>1080.9644798167631</v>
+        <v>1053.516959354966</v>
       </c>
       <c r="I11">
-        <v>-1197.695585453632</v>
+        <v>-1149.707600775173</v>
       </c>
       <c r="J11">
-        <v>1486.4837123660429</v>
+        <v>1558.039237948055</v>
       </c>
       <c r="K11">
-        <v>2184.5561305465048</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2157.033298989687</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>10</v>
       </c>
@@ -876,25 +821,25 @@
         <v>162.142</v>
       </c>
       <c r="F12">
-        <v>141.85330240318359</v>
+        <v>135.5025085979326</v>
       </c>
       <c r="G12">
-        <v>-49.573645376301911</v>
+        <v>-50.81158378858586</v>
       </c>
       <c r="H12">
-        <v>1170.34702441493</v>
+        <v>1138.818869393986</v>
       </c>
       <c r="I12">
-        <v>-1136.5322693738169</v>
+        <v>-1132.161097084835</v>
       </c>
       <c r="J12">
-        <v>1530.5106682875189</v>
+        <v>1551.861012288439</v>
       </c>
       <c r="K12">
-        <v>2325.0697052613618</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2296.485779119064</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>10</v>
       </c>
@@ -911,25 +856,25 @@
         <v>163.142</v>
       </c>
       <c r="F13">
-        <v>122.1847541855247</v>
+        <v>125.9777894241739</v>
       </c>
       <c r="G13">
-        <v>-34.404617707225832</v>
+        <v>-35.52017499769057</v>
       </c>
       <c r="H13">
-        <v>1208.9651710713961</v>
+        <v>1201.26963436906</v>
       </c>
       <c r="I13">
-        <v>-1156.990747897981</v>
+        <v>-1133.120684844117</v>
       </c>
       <c r="J13">
-        <v>1529.4420835291501</v>
+        <v>1491.83812608717</v>
       </c>
       <c r="K13">
-        <v>2529.0069977050111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2588.708153379439</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>10</v>
       </c>
@@ -946,25 +891,25 @@
         <v>164.142</v>
       </c>
       <c r="F14">
-        <v>110.9717418412606</v>
+        <v>108.8137119899331</v>
       </c>
       <c r="G14">
-        <v>-17.557212044523041</v>
+        <v>-17.93265580991357</v>
       </c>
       <c r="H14">
-        <v>1391.7905677469089</v>
+        <v>1373.046654434757</v>
       </c>
       <c r="I14">
-        <v>-1117.9440749256009</v>
+        <v>-1048.357573851607</v>
       </c>
       <c r="J14">
-        <v>1350.932188724398</v>
+        <v>1374.603933296502</v>
       </c>
       <c r="K14">
-        <v>2719.2724970511672</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2542.237801879255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>10</v>
       </c>
@@ -981,25 +926,25 @@
         <v>165.142</v>
       </c>
       <c r="F15">
-        <v>99.066542877629658</v>
+        <v>97.16514177430021</v>
       </c>
       <c r="G15">
-        <v>-0.95644092788593671</v>
+        <v>-0.9272430183320194</v>
       </c>
       <c r="H15">
-        <v>1322.415224013482</v>
+        <v>1433.209937748604</v>
       </c>
       <c r="I15">
-        <v>-1047.055406938231</v>
+        <v>-1079.864639739991</v>
       </c>
       <c r="J15">
-        <v>1426.666959091476</v>
+        <v>1412.118024637207</v>
       </c>
       <c r="K15">
-        <v>2829.1390076275138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2692.415232840783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1016,25 +961,25 @@
         <v>166.142</v>
       </c>
       <c r="F16">
-        <v>93.770648538702986</v>
+        <v>95.0376479819716</v>
       </c>
       <c r="G16">
-        <v>16.083491496683799</v>
+        <v>15.04665370881238</v>
       </c>
       <c r="H16">
-        <v>1431.0503916922719</v>
+        <v>1473.757472820108</v>
       </c>
       <c r="I16">
-        <v>-1040.952355850136</v>
+        <v>-1029.855452813576</v>
       </c>
       <c r="J16">
-        <v>1332.5677094038811</v>
+        <v>1358.765190820968</v>
       </c>
       <c r="K16">
-        <v>2811.6786151206989</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2752.217806083632</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1051,25 +996,25 @@
         <v>167.142</v>
       </c>
       <c r="F17">
-        <v>82.654840374239186</v>
+        <v>83.86022768392645</v>
       </c>
       <c r="G17">
-        <v>33.609527451429258</v>
+        <v>32.43582364564039</v>
       </c>
       <c r="H17">
-        <v>1487.692627169645</v>
+        <v>1517.484774530964</v>
       </c>
       <c r="I17">
-        <v>-985.8909847934051</v>
+        <v>-972.4725874756493</v>
       </c>
       <c r="J17">
-        <v>1232.2295233225359</v>
+        <v>1296.700922999422</v>
       </c>
       <c r="K17">
-        <v>2957.8976065345519</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2830.80735934923</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1086,25 +1031,25 @@
         <v>168.142</v>
       </c>
       <c r="F18">
-        <v>81.575877001681292</v>
+        <v>84.0914106364835</v>
       </c>
       <c r="G18">
-        <v>48.635229365080747</v>
+        <v>50.60315086276741</v>
       </c>
       <c r="H18">
-        <v>1457.556355202325</v>
+        <v>1517.286868442979</v>
       </c>
       <c r="I18">
-        <v>-945.45968845220386</v>
+        <v>-930.3109081275181</v>
       </c>
       <c r="J18">
-        <v>1274.523467259819</v>
+        <v>1265.287044781204</v>
       </c>
       <c r="K18">
-        <v>3142.9602282402579</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2967.366618984558</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1121,25 +1066,25 @@
         <v>169.142</v>
       </c>
       <c r="F19">
-        <v>77.250111788513124</v>
+        <v>77.14993120963955</v>
       </c>
       <c r="G19">
-        <v>62.17487388635508</v>
+        <v>68.36065919075436</v>
       </c>
       <c r="H19">
-        <v>1604.249218560662</v>
+        <v>1609.370432021196</v>
       </c>
       <c r="I19">
-        <v>-888.5553059710727</v>
+        <v>-917.9196239894678</v>
       </c>
       <c r="J19">
-        <v>1124.4590181958779</v>
+        <v>1146.81149391931</v>
       </c>
       <c r="K19">
-        <v>3200.5106703898932</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3080.519679385576</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1156,25 +1101,25 @@
         <v>170.142</v>
       </c>
       <c r="F20">
-        <v>76.438576920175123</v>
+        <v>72.56724459481697</v>
       </c>
       <c r="G20">
-        <v>82.008633972978544</v>
+        <v>80.48910240999909</v>
       </c>
       <c r="H20">
-        <v>1568.524882510545</v>
+        <v>1624.304792001691</v>
       </c>
       <c r="I20">
-        <v>-868.37814253108991</v>
+        <v>-835.5675167022373</v>
       </c>
       <c r="J20">
-        <v>1136.4302634513731</v>
+        <v>1170.684548364667</v>
       </c>
       <c r="K20">
-        <v>3279.002294674659</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3305.537146197419</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1191,25 +1136,25 @@
         <v>171.142</v>
       </c>
       <c r="F21">
-        <v>67.469949014071304</v>
+        <v>73.4220561295961</v>
       </c>
       <c r="G21">
-        <v>102.04867797263201</v>
+        <v>102.2675630366356</v>
       </c>
       <c r="H21">
-        <v>1617.4674915950741</v>
+        <v>1519.438986011786</v>
       </c>
       <c r="I21">
-        <v>-801.68780881531882</v>
+        <v>-826.2366436796773</v>
       </c>
       <c r="J21">
-        <v>1070.168034837769</v>
+        <v>1037.549698869207</v>
       </c>
       <c r="K21">
-        <v>3196.831807044643</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3162.39779882563</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>10</v>
       </c>
@@ -1226,25 +1171,25 @@
         <v>172.142</v>
       </c>
       <c r="F22">
-        <v>67.107588603480608</v>
+        <v>67.40996575937851</v>
       </c>
       <c r="G22">
-        <v>109.7453936728795</v>
+        <v>109.4615750148627</v>
       </c>
       <c r="H22">
-        <v>1664.039033448385</v>
+        <v>1562.499800235611</v>
       </c>
       <c r="I22">
-        <v>-772.64935834099776</v>
+        <v>-739.4842570105152</v>
       </c>
       <c r="J22">
-        <v>989.00239716696433</v>
+        <v>998.6149675804322</v>
       </c>
       <c r="K22">
-        <v>3109.5478161371452</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3326.341842740402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>10</v>
       </c>
@@ -1261,25 +1206,25 @@
         <v>173.142</v>
       </c>
       <c r="F23">
-        <v>64.546618963550955</v>
+        <v>64.83081221207055</v>
       </c>
       <c r="G23">
-        <v>126.4544995946401</v>
+        <v>124.7042453560242</v>
       </c>
       <c r="H23">
-        <v>1594.9317036725299</v>
+        <v>1665.042612561411</v>
       </c>
       <c r="I23">
-        <v>-722.16440289811271</v>
+        <v>-728.0077785379316</v>
       </c>
       <c r="J23">
-        <v>1024.072100385046</v>
+        <v>975.0441390031242</v>
       </c>
       <c r="K23">
-        <v>3261.494186741586</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3159.744436085696</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>10</v>
       </c>
@@ -1296,25 +1241,25 @@
         <v>174.142</v>
       </c>
       <c r="F24">
-        <v>63.251942926716303</v>
+        <v>63.1802633891307</v>
       </c>
       <c r="G24">
-        <v>144.33446512647731</v>
+        <v>150.1183885284138</v>
       </c>
       <c r="H24">
-        <v>1675.018589283846</v>
+        <v>1659.004501227952</v>
       </c>
       <c r="I24">
-        <v>-674.73774733259529</v>
+        <v>-668.9295348875107</v>
       </c>
       <c r="J24">
-        <v>965.17829650253339</v>
+        <v>968.8021631323185</v>
       </c>
       <c r="K24">
-        <v>3263.2637525953792</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3262.298105924876</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>10</v>
       </c>
@@ -1331,25 +1276,25 @@
         <v>175.142</v>
       </c>
       <c r="F25">
-        <v>64.526705032970469</v>
+        <v>61.63080937766918</v>
       </c>
       <c r="G25">
-        <v>169.3367007761139</v>
+        <v>163.5325562138718</v>
       </c>
       <c r="H25">
-        <v>1592.8854374258849</v>
+        <v>1608.356322625348</v>
       </c>
       <c r="I25">
-        <v>-607.61311103542562</v>
+        <v>-604.8531176186052</v>
       </c>
       <c r="J25">
-        <v>864.72460936350387</v>
+        <v>884.4884851397809</v>
       </c>
       <c r="K25">
-        <v>3167.608202073658</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3013.043544235238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>10</v>
       </c>
@@ -1366,25 +1311,25 @@
         <v>176.142</v>
       </c>
       <c r="F26">
-        <v>62.492728474847553</v>
+        <v>62.58686461344141</v>
       </c>
       <c r="G26">
-        <v>184.71738225341809</v>
+        <v>178.8615675588663</v>
       </c>
       <c r="H26">
-        <v>1628.9659123657691</v>
+        <v>1639.750305612225</v>
       </c>
       <c r="I26">
-        <v>-542.70796522527883</v>
+        <v>-564.7562781827546</v>
       </c>
       <c r="J26">
-        <v>841.57269303720045</v>
+        <v>852.5463912914187</v>
       </c>
       <c r="K26">
-        <v>2977.9101438553021</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3013.862997564465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1401,25 +1346,25 @@
         <v>177.142</v>
       </c>
       <c r="F27">
-        <v>60.566590349034122</v>
+        <v>56.26666101855694</v>
       </c>
       <c r="G27">
-        <v>187.4765921454823</v>
+        <v>191.9831184962643</v>
       </c>
       <c r="H27">
-        <v>1624.8723047660169</v>
+        <v>1778.909223390443</v>
       </c>
       <c r="I27">
-        <v>-469.19758802578372</v>
+        <v>-469.2806652837993</v>
       </c>
       <c r="J27">
-        <v>815.66139677319882</v>
+        <v>750.7508224323747</v>
       </c>
       <c r="K27">
-        <v>3153.0388679689481</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3013.622284439266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1436,25 +1381,25 @@
         <v>178.142</v>
       </c>
       <c r="F28">
-        <v>53.919971942601002</v>
+        <v>55.24259954684857</v>
       </c>
       <c r="G28">
-        <v>206.22988126833869</v>
+        <v>205.823114049112</v>
       </c>
       <c r="H28">
-        <v>1709.531442916302</v>
+        <v>1763.919186510255</v>
       </c>
       <c r="I28">
-        <v>-439.8465676722189</v>
+        <v>-431.5266897928079</v>
       </c>
       <c r="J28">
-        <v>704.30549241534504</v>
+        <v>756.6536976333118</v>
       </c>
       <c r="K28">
-        <v>3052.0028034286561</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3022.379307873263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1471,25 +1416,25 @@
         <v>179.142</v>
       </c>
       <c r="F29">
-        <v>55.079357765148423</v>
+        <v>55.7312258905984</v>
       </c>
       <c r="G29">
-        <v>241.6795197865961</v>
+        <v>227.1513508602628</v>
       </c>
       <c r="H29">
-        <v>1742.3862514836121</v>
+        <v>1717.069377541605</v>
       </c>
       <c r="I29">
-        <v>-382.00889773964713</v>
+        <v>-384.9474775797055</v>
       </c>
       <c r="J29">
-        <v>654.35628124489938</v>
+        <v>697.4519118298657</v>
       </c>
       <c r="K29">
-        <v>2964.870537859279</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2971.474591042006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1506,25 +1451,25 @@
         <v>180.142</v>
       </c>
       <c r="F30">
-        <v>53.197419555725233</v>
+        <v>54.2009096789393</v>
       </c>
       <c r="G30">
-        <v>240.10873623252311</v>
+        <v>247.2022455247485</v>
       </c>
       <c r="H30">
-        <v>1786.691129712083</v>
+        <v>1756.684406085497</v>
       </c>
       <c r="I30">
-        <v>-315.67228330528769</v>
+        <v>-326.0826901213546</v>
       </c>
       <c r="J30">
-        <v>668.02072886284816</v>
+        <v>643.3520015533271</v>
       </c>
       <c r="K30">
-        <v>2692.6660355094568</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2865.962401643062</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1541,25 +1486,25 @@
         <v>181.142</v>
       </c>
       <c r="F31">
-        <v>53.168035402288787</v>
+        <v>53.33409439551652</v>
       </c>
       <c r="G31">
-        <v>263.46081870904447</v>
+        <v>258.4038732918999</v>
       </c>
       <c r="H31">
-        <v>1851.499834984369</v>
+        <v>1843.475823401016</v>
       </c>
       <c r="I31">
-        <v>-268.24715181396789</v>
+        <v>-259.1936021000882</v>
       </c>
       <c r="J31">
-        <v>575.92728814602003</v>
+        <v>582.1825361082961</v>
       </c>
       <c r="K31">
-        <v>2736.8994001535671</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2750.254298656001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>10</v>
       </c>
@@ -1576,25 +1521,25 @@
         <v>182.142</v>
       </c>
       <c r="F32">
-        <v>50.948053207163547</v>
+        <v>51.14893594462347</v>
       </c>
       <c r="G32">
-        <v>281.62985029574048</v>
+        <v>278.1865803335052</v>
       </c>
       <c r="H32">
-        <v>1718.239647143602</v>
+        <v>1846.345310508557</v>
       </c>
       <c r="I32">
-        <v>-214.90843281841131</v>
+        <v>-211.5455727023748</v>
       </c>
       <c r="J32">
-        <v>527.48974615074758</v>
+        <v>538.5599070818739</v>
       </c>
       <c r="K32">
-        <v>2435.15438295696</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2523.042089744286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>10</v>
       </c>
@@ -1611,25 +1556,25 @@
         <v>183.142</v>
       </c>
       <c r="F33">
-        <v>52.121594540046686</v>
+        <v>47.86013926859631</v>
       </c>
       <c r="G33">
-        <v>302.75585699571371</v>
+        <v>296.2702573734949</v>
       </c>
       <c r="H33">
-        <v>1769.490381722414</v>
+        <v>1735.513290767555</v>
       </c>
       <c r="I33">
-        <v>-150.3468767208598</v>
+        <v>-143.0867045217527</v>
       </c>
       <c r="J33">
-        <v>504.67134108328628</v>
+        <v>474.4350986069132</v>
       </c>
       <c r="K33">
-        <v>2480.6967955140849</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2316.70848125954</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1646,25 +1591,25 @@
         <v>184.142</v>
       </c>
       <c r="F34">
-        <v>50.870382336247623</v>
+        <v>48.08447459670824</v>
       </c>
       <c r="G34">
-        <v>299.64409014064159</v>
+        <v>320.7417843608654</v>
       </c>
       <c r="H34">
-        <v>1869.3812360726811</v>
+        <v>1874.890501178554</v>
       </c>
       <c r="I34">
-        <v>-83.233765108324008</v>
+        <v>-81.55379439407463</v>
       </c>
       <c r="J34">
-        <v>451.33453053435892</v>
+        <v>445.8248920925536</v>
       </c>
       <c r="K34">
-        <v>2105.8404462325502</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2127.869655760593</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>10</v>
       </c>
@@ -1681,25 +1626,25 @@
         <v>185.142</v>
       </c>
       <c r="F35">
-        <v>45.87699679367514</v>
+        <v>50.11461017445732</v>
       </c>
       <c r="G35">
-        <v>345.534252534583</v>
+        <v>339.6937687209411</v>
       </c>
       <c r="H35">
-        <v>1843.9487379006121</v>
+        <v>1827.072596905194</v>
       </c>
       <c r="I35">
-        <v>-18.546406177933701</v>
+        <v>-18.8021453904238</v>
       </c>
       <c r="J35">
-        <v>393.32529468494698</v>
+        <v>388.6882307881807</v>
       </c>
       <c r="K35">
-        <v>1985.384410353659</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2109.321354599191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>10</v>
       </c>
@@ -1716,25 +1661,25 @@
         <v>186.142</v>
       </c>
       <c r="F36">
-        <v>48.776564927215233</v>
+        <v>48.28831298898171</v>
       </c>
       <c r="G36">
-        <v>357.38607269942622</v>
+        <v>329.1138020145842</v>
       </c>
       <c r="H36">
-        <v>1872.2554731687731</v>
+        <v>1879.760248352524</v>
       </c>
       <c r="I36">
-        <v>45.604849952874858</v>
+        <v>47.81067205418263</v>
       </c>
       <c r="J36">
-        <v>330.2846387260484</v>
+        <v>355.7863393530487</v>
       </c>
       <c r="K36">
-        <v>1906.018515128718</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1885.795265415969</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>10</v>
       </c>
@@ -1751,25 +1696,25 @@
         <v>187.142</v>
       </c>
       <c r="F37">
-        <v>45.653873603766002</v>
+        <v>47.79981952004732</v>
       </c>
       <c r="G37">
-        <v>371.55843537997839</v>
+        <v>379.0314156394633</v>
       </c>
       <c r="H37">
-        <v>1753.994945621926</v>
+        <v>1924.86257015555</v>
       </c>
       <c r="I37">
-        <v>112.9418738447889</v>
+        <v>109.9941218001605</v>
       </c>
       <c r="J37">
-        <v>290.09475987286498</v>
+        <v>284.4640032178323</v>
       </c>
       <c r="K37">
-        <v>1591.4496645864469</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1584.231826597959</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>10</v>
       </c>
@@ -1786,25 +1731,25 @@
         <v>188.142</v>
       </c>
       <c r="F38">
-        <v>43.895399075925212</v>
+        <v>47.6639504378576</v>
       </c>
       <c r="G38">
-        <v>378.88785280424707</v>
+        <v>391.4796257987088</v>
       </c>
       <c r="H38">
-        <v>1791.2652705000651</v>
+        <v>1823.285224249025</v>
       </c>
       <c r="I38">
-        <v>188.0757921633913</v>
+        <v>177.7184092596517</v>
       </c>
       <c r="J38">
-        <v>236.88015558565451</v>
+        <v>238.251611322319</v>
       </c>
       <c r="K38">
-        <v>1339.705260906481</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1401.195069036983</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>10</v>
       </c>
@@ -1821,25 +1766,25 @@
         <v>189.142</v>
       </c>
       <c r="F39">
-        <v>45.070712506055912</v>
+        <v>43.33049225929747</v>
       </c>
       <c r="G39">
-        <v>397.55019008857232</v>
+        <v>392.8997930222339</v>
       </c>
       <c r="H39">
-        <v>1847.3936716790961</v>
+        <v>1951.376746322633</v>
       </c>
       <c r="I39">
-        <v>252.22881063625579</v>
+        <v>258.4524330146502</v>
       </c>
       <c r="J39">
-        <v>190.19938801028661</v>
+        <v>198.6479027168259</v>
       </c>
       <c r="K39">
-        <v>1208.402032877018</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1130.105288927545</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>10</v>
       </c>
@@ -1856,25 +1801,25 @@
         <v>190.142</v>
       </c>
       <c r="F40">
-        <v>43.886698018924051</v>
+        <v>42.13801051890773</v>
       </c>
       <c r="G40">
-        <v>402.73919822588101</v>
+        <v>423.4515587681851</v>
       </c>
       <c r="H40">
-        <v>1958.892637199529</v>
+        <v>1924.205420819199</v>
       </c>
       <c r="I40">
-        <v>318.18384030506962</v>
+        <v>324.4187085382803</v>
       </c>
       <c r="J40">
-        <v>155.60648960622009</v>
+        <v>146.3572481880372</v>
       </c>
       <c r="K40">
-        <v>877.86692965063389</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>923.7650330577743</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>10</v>
       </c>
@@ -1891,25 +1836,25 @@
         <v>191.142</v>
       </c>
       <c r="F41">
-        <v>41.35089972086395</v>
+        <v>41.88782168883781</v>
       </c>
       <c r="G41">
-        <v>428.67894984521092</v>
+        <v>437.073735378574</v>
       </c>
       <c r="H41">
-        <v>1853.337582596333</v>
+        <v>1943.937846658554</v>
       </c>
       <c r="I41">
-        <v>400.71939299968841</v>
+        <v>389.979689438239</v>
       </c>
       <c r="J41">
-        <v>97.971194699994243</v>
+        <v>104.6519145021644</v>
       </c>
       <c r="K41">
-        <v>614.95086158181095</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>641.2664451964006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>10</v>
       </c>
@@ -1926,25 +1871,25 @@
         <v>192.142</v>
       </c>
       <c r="F42">
-        <v>41.959200820446711</v>
+        <v>41.54909578175238</v>
       </c>
       <c r="G42">
-        <v>434.49856116937781</v>
+        <v>448.7645098379222</v>
       </c>
       <c r="H42">
-        <v>1888.845001107728</v>
+        <v>1857.696679748807</v>
       </c>
       <c r="I42">
-        <v>492.12628172851959</v>
+        <v>460.5733813255522</v>
       </c>
       <c r="J42">
-        <v>52.290361631941117</v>
+        <v>52.88020524242419</v>
       </c>
       <c r="K42">
-        <v>335.24504236646158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>350.3264467730222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>10</v>
       </c>
@@ -1961,25 +1906,25 @@
         <v>193.142</v>
       </c>
       <c r="F43">
-        <v>42.222625404389007</v>
+        <v>41.89318297376273</v>
       </c>
       <c r="G43">
-        <v>450.04943829787248</v>
+        <v>456.7422771869212</v>
       </c>
       <c r="H43">
-        <v>1928.1917810650009</v>
+        <v>1817.072769628431</v>
       </c>
       <c r="I43">
-        <v>555.3458148686741</v>
+        <v>542.6650117726352</v>
       </c>
       <c r="J43">
-        <v>5.1386704415449733</v>
+        <v>5.361397967670222</v>
       </c>
       <c r="K43">
-        <v>33.41669394809616</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34.25526678138262</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>10</v>
       </c>
@@ -1996,25 +1941,25 @@
         <v>194.142</v>
       </c>
       <c r="F44">
-        <v>41.355047289791081</v>
+        <v>41.17604920802057</v>
       </c>
       <c r="G44">
-        <v>485.71452451474357</v>
+        <v>479.5489392116456</v>
       </c>
       <c r="H44">
-        <v>1902.3242502739811</v>
+        <v>1998.206049079525</v>
       </c>
       <c r="I44">
-        <v>633.24052336082752</v>
+        <v>612.0289528457338</v>
       </c>
       <c r="J44">
-        <v>-42.680836923400378</v>
+        <v>-42.84872516041617</v>
       </c>
       <c r="K44">
-        <v>-277.76364971895282</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-285.7778212118015</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>10</v>
       </c>
@@ -2031,25 +1976,25 @@
         <v>195.142</v>
       </c>
       <c r="F45">
-        <v>42.449999387201402</v>
+        <v>42.70933018626154</v>
       </c>
       <c r="G45">
-        <v>495.42869437702018</v>
+        <v>482.1518819180341</v>
       </c>
       <c r="H45">
-        <v>1823.069404416842</v>
+        <v>2010.659565174453</v>
       </c>
       <c r="I45">
-        <v>701.15148658469911</v>
+        <v>726.0760812229324</v>
       </c>
       <c r="J45">
-        <v>-96.140251261150851</v>
+        <v>-96.36146026552343</v>
       </c>
       <c r="K45">
-        <v>-625.59871938878484</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-600.1224731447538</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>10</v>
       </c>
@@ -2066,25 +2011,25 @@
         <v>196.142</v>
       </c>
       <c r="F46">
-        <v>40.217900168550791</v>
+        <v>40.55609759288938</v>
       </c>
       <c r="G46">
-        <v>509.84984475235348</v>
+        <v>489.2042498473633</v>
       </c>
       <c r="H46">
-        <v>1973.865050456378</v>
+        <v>1986.903597143377</v>
       </c>
       <c r="I46">
-        <v>794.88722781694605</v>
+        <v>797.164044024795</v>
       </c>
       <c r="J46">
-        <v>-144.90040805940561</v>
+        <v>-143.0097966233286</v>
       </c>
       <c r="K46">
-        <v>-932.89029757615424</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-928.2759554518835</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2101,25 +2046,25 @@
         <v>197.142</v>
       </c>
       <c r="F47">
-        <v>38.336982644975947</v>
+        <v>40.95919789406019</v>
       </c>
       <c r="G47">
-        <v>533.33072788473658</v>
+        <v>553.7571020219625</v>
       </c>
       <c r="H47">
-        <v>1896.976113312965</v>
+        <v>1945.752895090712</v>
       </c>
       <c r="I47">
-        <v>898.68503724404752</v>
+        <v>854.4317315580778</v>
       </c>
       <c r="J47">
-        <v>-194.6283848765604</v>
+        <v>-182.1968072400078</v>
       </c>
       <c r="K47">
-        <v>-1345.096550223021</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-1364.526466426827</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>10</v>
       </c>
@@ -2136,25 +2081,25 @@
         <v>198.142</v>
       </c>
       <c r="F48">
-        <v>40.843275103863789</v>
+        <v>37.52636691283905</v>
       </c>
       <c r="G48">
-        <v>569.39319505331616</v>
+        <v>536.0614554507888</v>
       </c>
       <c r="H48">
-        <v>1944.216138447126</v>
+        <v>1926.139173043984</v>
       </c>
       <c r="I48">
-        <v>963.40381741739691</v>
+        <v>965.4963202540315</v>
       </c>
       <c r="J48">
-        <v>-226.75011433993839</v>
+        <v>-239.5173826112327</v>
       </c>
       <c r="K48">
-        <v>-1715.6778484516769</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-1619.802140270479</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>10</v>
       </c>
@@ -2171,25 +2116,25 @@
         <v>199.142</v>
       </c>
       <c r="F49">
-        <v>38.302557243291439</v>
+        <v>38.66060522638427</v>
       </c>
       <c r="G49">
-        <v>587.73332933864117</v>
+        <v>550.2982288724132</v>
       </c>
       <c r="H49">
-        <v>1851.215989570891</v>
+        <v>1999.94183371625</v>
       </c>
       <c r="I49">
-        <v>1101.7757502244881</v>
+        <v>1074.276413224097</v>
       </c>
       <c r="J49">
-        <v>-293.84812067120782</v>
+        <v>-292.0187023387205</v>
       </c>
       <c r="K49">
-        <v>-2183.1741982318708</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-2033.572535229269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>10</v>
       </c>
@@ -2206,25 +2151,25 @@
         <v>200.142</v>
       </c>
       <c r="F50">
-        <v>37.265958935030213</v>
+        <v>38.98551191513928</v>
       </c>
       <c r="G50">
-        <v>591.28752167349955</v>
+        <v>594.2045531338352</v>
       </c>
       <c r="H50">
-        <v>1900.5424954021939</v>
+        <v>1915.621131728892</v>
       </c>
       <c r="I50">
-        <v>1114.7172654307569</v>
+        <v>1198.05913088838</v>
       </c>
       <c r="J50">
-        <v>-347.4927348222401</v>
+        <v>-329.7875744744806</v>
       </c>
       <c r="K50">
-        <v>-2518.8623784098991</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-2626.990404955229</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>10</v>
       </c>
@@ -2241,25 +2186,25 @@
         <v>201.142</v>
       </c>
       <c r="F51">
-        <v>39.060771648544993</v>
+        <v>37.56319192394465</v>
       </c>
       <c r="G51">
-        <v>602.32190483886836</v>
+        <v>602.2286129535896</v>
       </c>
       <c r="H51">
-        <v>2044.466437002367</v>
+        <v>1926.851098652049</v>
       </c>
       <c r="I51">
-        <v>1257.137786133218</v>
+        <v>1268.506647824257</v>
       </c>
       <c r="J51">
-        <v>-367.75986478594899</v>
+        <v>-392.962752026836</v>
       </c>
       <c r="K51">
-        <v>-3049.0627047571779</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-2806.258746610545</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>10</v>
       </c>
@@ -2276,25 +2221,25 @@
         <v>202.142</v>
       </c>
       <c r="F52">
-        <v>36.106114052652373</v>
+        <v>38.44200368650287</v>
       </c>
       <c r="G52">
-        <v>589.77779488066801</v>
+        <v>615.0782367611706</v>
       </c>
       <c r="H52">
-        <v>1922.740840742506</v>
+        <v>1978.751076569446</v>
       </c>
       <c r="I52">
-        <v>1351.943833234119</v>
+        <v>1369.87656717986</v>
       </c>
       <c r="J52">
-        <v>-439.99219940936052</v>
+        <v>-430.4182254480932</v>
       </c>
       <c r="K52">
-        <v>-3298.8324688380271</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3312.146965076264</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>10</v>
       </c>
@@ -2311,25 +2256,25 @@
         <v>203.142</v>
       </c>
       <c r="F53">
-        <v>35.370717954915243</v>
+        <v>35.533018767313</v>
       </c>
       <c r="G53">
-        <v>609.90828523846346</v>
+        <v>614.0807706851593</v>
       </c>
       <c r="H53">
-        <v>2064.0217927580252</v>
+        <v>1907.568128332946</v>
       </c>
       <c r="I53">
-        <v>1474.038748246626</v>
+        <v>1465.528399736654</v>
       </c>
       <c r="J53">
-        <v>-504.38677971185069</v>
+        <v>-505.0886882008357</v>
       </c>
       <c r="K53">
-        <v>-3781.5554162721251</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3916.622400610061</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>10</v>
       </c>
@@ -2346,22 +2291,22 @@
         <v>204.142</v>
       </c>
       <c r="F54">
-        <v>37.591285576827033</v>
+        <v>36.95428884438494</v>
       </c>
       <c r="G54">
-        <v>634.19825544549542</v>
+        <v>672.0749758684442</v>
       </c>
       <c r="H54">
-        <v>1944.538960190622</v>
+        <v>2074.299614077109</v>
       </c>
       <c r="I54">
-        <v>1604.657845110235</v>
+        <v>1543.578363771924</v>
       </c>
       <c r="J54">
-        <v>-510.07629745654629</v>
+        <v>-516.7258378169637</v>
       </c>
       <c r="K54">
-        <v>-4255.5852029030393</v>
+        <v>-4284.99317888731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>